<commit_message>
list of methods used (Updated)
</commit_message>
<xml_diff>
--- a/MethodList.xlsx
+++ b/MethodList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duquet\Documents\GitHub\RENE_Track\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duquet\Documents\GitHub\RENE-PredictingMetamorphicRelations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -113,9 +113,6 @@
     <t>safeNorm</t>
   </si>
   <si>
-    <t>DistInf</t>
-  </si>
-  <si>
     <t>sampleKurtosis</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>lag</t>
   </si>
   <si>
-    <t>Dist</t>
-  </si>
-  <si>
     <t>square</t>
   </si>
   <si>
@@ -387,6 +381,12 @@
   </si>
   <si>
     <t>INV</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>distInf</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K1:K1048576"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,18 +738,18 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -761,31 +761,31 @@
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -793,16 +793,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -828,16 +828,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -863,16 +863,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -901,13 +901,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -936,13 +936,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -968,16 +968,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -1006,13 +1006,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -1038,16 +1038,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -1073,16 +1073,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
@@ -1111,13 +1111,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
@@ -1146,13 +1146,13 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
@@ -1181,13 +1181,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
@@ -1213,16 +1213,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
@@ -1248,16 +1248,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -1286,13 +1286,13 @@
         <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
@@ -1321,13 +1321,13 @@
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
@@ -1353,16 +1353,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" s="2">
         <v>0</v>
@@ -1391,13 +1391,13 @@
         <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" s="2">
         <v>0</v>
@@ -1423,16 +1423,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -1461,13 +1461,13 @@
         <v>18</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
@@ -1493,16 +1493,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>
@@ -1528,16 +1528,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
@@ -1566,13 +1566,13 @@
         <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
@@ -1601,13 +1601,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>
@@ -1633,16 +1633,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27" s="2">
         <v>1</v>
@@ -1668,16 +1668,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>
@@ -1703,16 +1703,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" s="2">
         <v>0</v>
@@ -1738,16 +1738,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" s="2">
         <v>1</v>
@@ -1773,16 +1773,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F31" s="2">
         <v>0</v>
@@ -1808,16 +1808,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F32" s="2">
         <v>1</v>
@@ -1843,16 +1843,16 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F33" s="2">
         <v>0</v>
@@ -1878,16 +1878,16 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F34" s="2">
         <v>1</v>
@@ -1913,16 +1913,16 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35" s="2">
         <v>0</v>
@@ -1948,16 +1948,16 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F36" s="2">
         <v>0</v>
@@ -1983,16 +1983,16 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
@@ -2018,16 +2018,16 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
@@ -2053,16 +2053,16 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F39" s="2">
         <v>0</v>
@@ -2088,16 +2088,16 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
@@ -2123,16 +2123,16 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F41" s="2">
         <v>0</v>
@@ -2158,16 +2158,16 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F42" s="2">
         <v>0</v>
@@ -2193,16 +2193,16 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F43" s="2">
         <v>0</v>
@@ -2228,16 +2228,16 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F44" s="2">
         <v>1</v>
@@ -2263,16 +2263,16 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F45" s="2">
         <v>0</v>
@@ -2298,16 +2298,16 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F46" s="2">
         <v>0</v>
@@ -2333,16 +2333,16 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F47" s="2">
         <v>1</v>
@@ -2368,16 +2368,16 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F48" s="2">
         <v>0</v>
@@ -2403,16 +2403,16 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F49" s="2">
         <v>0</v>
@@ -2438,16 +2438,16 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F50" s="2">
         <v>1</v>
@@ -2473,16 +2473,16 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F51" s="2">
         <v>1</v>
@@ -2508,16 +2508,16 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
@@ -2543,16 +2543,16 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F53" s="2">
         <v>1</v>
@@ -2578,16 +2578,16 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F54" s="2">
         <v>1</v>
@@ -2613,16 +2613,16 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F55" s="2">
         <v>0</v>
@@ -2648,16 +2648,16 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F56" s="2">
         <v>1</v>
@@ -2683,16 +2683,16 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F57" s="2">
         <v>1</v>
@@ -2718,16 +2718,16 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F58" s="2">
         <v>0</v>
@@ -2756,13 +2756,13 @@
         <v>3</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F59" s="2">
         <v>1</v>
@@ -2788,16 +2788,16 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F60" s="2">
         <v>1</v>
@@ -2826,13 +2826,13 @@
         <v>4</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F61" s="2">
         <v>1</v>
@@ -2858,16 +2858,16 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F62" s="2">
         <v>0</v>
@@ -2896,13 +2896,13 @@
         <v>7</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F63" s="2">
         <v>0</v>
@@ -2931,13 +2931,13 @@
         <v>9</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F64" s="2">
         <v>0</v>
@@ -2966,13 +2966,13 @@
         <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F65" s="2">
         <v>1</v>
@@ -3001,13 +3001,13 @@
         <v>11</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F66" s="2">
         <v>1</v>
@@ -3033,16 +3033,16 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F67" s="2">
         <v>0</v>
@@ -3068,16 +3068,16 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F68" s="2">
         <v>0</v>
@@ -3106,13 +3106,13 @@
         <v>14</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F69" s="2">
         <v>1</v>
@@ -3141,13 +3141,13 @@
         <v>16</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F70" s="2">
         <v>0</v>
@@ -3176,13 +3176,13 @@
         <v>17</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F71" s="2">
         <v>1</v>
@@ -3211,13 +3211,13 @@
         <v>19</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F72" s="2">
         <v>1</v>
@@ -3246,13 +3246,13 @@
         <v>20</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F73" s="2">
         <v>1</v>
@@ -3281,13 +3281,13 @@
         <v>21</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F74" s="2">
         <v>0</v>
@@ -3316,13 +3316,13 @@
         <v>23</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F75" s="2">
         <v>1</v>
@@ -3351,13 +3351,13 @@
         <v>25</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F76" s="2">
         <v>1</v>
@@ -3386,13 +3386,13 @@
         <v>26</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F77" s="2">
         <v>1</v>
@@ -3421,13 +3421,13 @@
         <v>27</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F78" s="2">
         <v>1</v>
@@ -3453,16 +3453,16 @@
         <v>77</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F79" s="2">
         <v>1</v>
@@ -3488,16 +3488,16 @@
         <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F80" s="2">
         <v>1</v>
@@ -3523,16 +3523,16 @@
         <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F81" s="2">
         <v>1</v>
@@ -3558,16 +3558,16 @@
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F82" s="2">
         <v>0</v>
@@ -3593,16 +3593,16 @@
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F83" s="2">
         <v>1</v>
@@ -3628,16 +3628,16 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F84" s="2">
         <v>1</v>
@@ -3663,16 +3663,16 @@
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F85" s="2">
         <v>1</v>
@@ -3698,16 +3698,16 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F86" s="2">
         <v>0</v>
@@ -3733,16 +3733,16 @@
         <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F87" s="2">
         <v>1</v>
@@ -3768,16 +3768,16 @@
         <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F88" s="2">
         <v>1</v>
@@ -3803,16 +3803,16 @@
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F89" s="2">
         <v>1</v>
@@ -3838,16 +3838,16 @@
         <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F90" s="2">
         <v>1</v>
@@ -3873,16 +3873,16 @@
         <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F91" s="2">
         <v>1</v>
@@ -3908,16 +3908,16 @@
         <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F92" s="2">
         <v>1</v>
@@ -3943,16 +3943,16 @@
         <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F93" s="2">
         <v>1</v>
@@ -3978,16 +3978,16 @@
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F94" s="2">
         <v>0</v>
@@ -4013,16 +4013,16 @@
         <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F95" s="2">
         <v>0</v>
@@ -4048,16 +4048,16 @@
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F96" s="2">
         <v>0</v>
@@ -4083,16 +4083,16 @@
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F97" s="2">
         <v>1</v>
@@ -4118,16 +4118,16 @@
         <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F98" s="2">
         <v>1</v>
@@ -4153,16 +4153,16 @@
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F99" s="2">
         <v>1</v>
@@ -4188,16 +4188,16 @@
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F100" s="2">
         <v>0</v>
@@ -4223,16 +4223,16 @@
         <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F101" s="2">
         <v>1</v>
@@ -4258,16 +4258,16 @@
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F102" s="2">
         <v>1</v>

</xml_diff>